<commit_message>
added results from groudingdino, added changes to pipeline/random subset creation only picks tweets with a gemini caption
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,7 +444,37 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>gemini_descriptionconfidence</t>
+          <t>gemini_description</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>facial_emotion</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>text_similarity_semantic</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>text_similarity_semantic_expression</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>labels</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>bounding_boxes</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>bounding_box_confidence</t>
         </is>
       </c>
     </row>
@@ -454,7 +484,11 @@
           <t>id_1153283149360762880_2019-07-22.jpg</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">poster, </t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>a screenshot of a cell phone with a message about the weather</t>
@@ -470,8 +504,29 @@
           <t xml:space="preserve"> The image is a screenshot of a web page. The web page is about the United Nations. The background of the web page is white. There is a blue bar at the top of the web page. The blue bar contains the words "Welcome to the United Nations" in white text. There is a gray bar below the blue bar. The gray bar contains the words "Language:" in black text. There is a drop-down menu next to the word "Language:". The drop-down menu contains a list of languages. The languages are listed in alphabetical order. The first language in the list is "العربية". The last language in the list is "Español". The image is a photo.</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>0.8735179106394449</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>0.8735178311665853</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>[    0.50049     0.50024     0.98844     0.99073]</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0.4777811</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -496,9 +551,22 @@
           <t xml:space="preserve"> There are 15 trees on the right side of the image.They are bare,and their branches are covered in snow.There is a large body of water, which is probably a frozen lake, in the middle of the image. There are some bushes and shrubs on the left side of the image.They are also covered in snow. There are footprints in the snow, which lead from the left side of the image to the right side. The background of the image is a clear blue sky. The setting of the image is a frozen lake in a forest. The image is a photo.</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
         <v>0.8720777829488119</v>
       </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -506,11 +574,7 @@
           <t>id_1122574040936452097_2019-04-28.jpg</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">bird, </t>
-        </is>
-      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
           <t>a close up of a hole in a wall with a black and white dog</t>
@@ -526,9 +590,22 @@
           <t xml:space="preserve"> This is an image of a hole in a wall. The hole is jagged and has a few pieces of debris around it. The wall is painted white. The background of the image is a wall painted white. The setting of the image is a room, most likely a bedroom. The type of image is a photo.</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>0.903128465016683</v>
-      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9031285444895426</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -556,8 +633,29 @@
           <t xml:space="preserve"> The image shows a man in a purple suit, green vest, and red pants falling down a snowy set of stairs. He has his arms in the air and his face is obscured by his hair. There is a street light at the top of the stairs and a wall on either side. The background is a dark sky. The image is a photo.</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>0.9182259241739908</v>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>disgust</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>0.9182257652282715</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>[    0.55928     0.55452     0.47864     0.57719]</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>0.5110339</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -568,7 +666,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">person, </t>
+          <t xml:space="preserve">tree, plant, </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -586,8 +684,29 @@
           <t xml:space="preserve"> The image is a cartoon. It shows a tree inside a glass dome. The tree has a few branches and yellow leaves. There is a brown squirrel sitting on one of the branches. There is a small blue house to the right of the tree. There are 5 pink jellyfish outside of the glass dome. There are 3 orange starfish on the sandy ground. The background is light blue with some purple and pink flowers.</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>0.9083538850148519</v>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>surprise</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>0.9083539644877116</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>[     0.4836      0.4533     0.31186     0.37395],[    0.48356     0.45354     0.30985      0.3733]</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0.6861728, 0.43398994</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -616,8 +735,29 @@
           <t xml:space="preserve"> This is a photo of a man sitting at a desk with his hand on his face. He is wearing a dark colored outfit. There is a candle on the desk, as well as some papers. The background of the image is a dark colored wall with a wooden door. The setting of the background is a room in a castle or other type of large building. The image is a still from the TV show Game of Thrones.</t>
         </is>
       </c>
-      <c r="F7" t="n">
-        <v>0.8902325630187988</v>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>disgust</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>0.8902324835459391</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>[    0.64667     0.47426     0.59342     0.71294]</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>0.51144177</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -628,7 +768,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">book, person, </t>
+          <t xml:space="preserve">poster, </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -646,8 +786,33 @@
           <t xml:space="preserve"> The image shows a bronze plaque with Icelandic and English text mounted on a large rock.The Icelandic text reads: "Bréf til framtíðarinnar" and the English text reads: "A letter to the future." Below the text, there is a date that reads: "Ágúst 2019" and below that, there are numbers that read "415ppm CO2". In the background, there is a group of about one hundred people dressed in warm clothes and standing on a rocky glacier. There is snow on the ground and in the distance there are snow-covered mountains. The image is a photograph.</t>
         </is>
       </c>
-      <c r="F8" t="n">
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>happy</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
         <v>0.9210977554321289</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>crowded</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>[    0.25319     0.52039     0.50318     0.94886]</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>0.57296276</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -658,7 +823,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">person, couch, </t>
+          <t xml:space="preserve">person, poster, </t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -676,8 +841,29 @@
           <t xml:space="preserve"> The image is a photo of Michael Scott from the TV show The Office. He is sitting on a couch in the break room at work. He is wearing a light blue shirt and dark grey pants. He has a tie on but it is undone and draped around his neck. He is sitting with his legs crossed and his hands in the air. He is looking at the camera with a surprised expression on his face. There is a coffee table in front of him with a newspaper on it. There is a painting on the wall behind him of a mountain landscape. The background of the image is the break room at work. It is an indoor setting. The image is a still frame from the TV show.</t>
         </is>
       </c>
-      <c r="F9" t="n">
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>surprise</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
         <v>0.8911571502685547</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>[    0.48131     0.56876     0.58897     0.85699],[    0.42381     0.18348     0.55205     0.36521]</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>0.49001718, 0.38414583</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -686,7 +872,11 @@
           <t>id_1163810197778903040_2019-08-20.jpg</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tree, </t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>smoke billowing from a forest fire in the middle of the day</t>
@@ -702,8 +892,343 @@
           <t xml:space="preserve"> The image shows a forest fire. The fire is burning in the middle of the forest. The trees are green and lush. The fire is orange and yellow. The smoke from the fire is white and gray. The smoke is billowing up into the sky. There are no people or animals visible in the image. The background of the image is a forest. The setting of the background is a jungle. The image is a photo.</t>
         </is>
       </c>
-      <c r="F10" t="n">
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
         <v>0.9032729466756185</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>[     0.4997     0.75507     0.99399     0.48348]</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>0.41401386</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>id_1104737401602228225_2019-03-10.jpg</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">person, </t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>there is a man standing on a rock in the woods</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>A man stands confidently on a rocky cliff, his gaze directed towards the camera. He is dressed in a blue shirt and sunglasses, and the cliff is surrounded by a lush forest of tall trees with green leaves. The man's position on the cliff and the verdant forest create a sense of depth and perspective in the image.</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> This is a photo of a man standing in a forest. The man is in his 40s, with dark hair and brown eyes. He is wearing a blue shirt and sunglasses. He has a friendly expression on his face. The forest is dense, with tall trees and a thick understory. The trees are mostly green, but there are a few yellow and orange leaves. The ground is covered in leaves and moss. There is a small stream in the background. The photo was taken on a sunny day. The background of the photo is a mountain range. The mountains are covered in snow. The photo is taken from a slightly elevated perspective.</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>disgust</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>0.9049077033996582</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>[    0.21827     0.69374     0.43625     0.61303]</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>0.6026033</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>id_1092817526399078400_2019-02-05.jpg</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">poster, person, </t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>arafed audience of students in a gymnasium watching a man on a stage</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>The image depicts a lively scene in a gymnasium, with a group of people gathered in front of a stage. The stage is adorned with a large banner displaying the words "Founded in 1892" and "New York City", suggesting it is a significant event. The gymnasium is filled with people, some sitting on the floor and others standing, all engaged in the event. The perspective of the image is from the back of the gymnasium, providing a comprehensive view of the scene.</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> This is a photo of a group of girls in a gym. There are about 100 girls sitting on the bleachers. They are all wearing school uniforms. There is one girl standing in front of the bleachers. She is wearing a black suit. She is holding hands with another girl who is sitting on the bleachers. The girl in the black suit is smiling. The girl sitting on the bleachers is also smiling. The background of the photo is a stage. There is a red curtain behind the stage. There are some chairs on the stage. There is a podium on the stage. There is a banner hanging from the ceiling. The banner has the words "The Young Women's Leadership School" on it.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>sadness</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>0.8510868549346924</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>crowded</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>[    0.81833      0.3493     0.23254     0.59861],[     0.5434     0.43226     0.17948     0.30161]</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>0.4040551, 0.4006823</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>id_1161027544096923656_2019-08-12.jpg</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">person, tree, </t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>arafed man taking a picture of himself in a garden</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>A young man stands in a lush garden, his hands raised to his face as if in deep thought. He is dressed casually in a gray t-shirt and blue shorts. The garden is a vibrant display of nature, with a variety of flowers and plants in shades of green, purple, and white. The man is positioned in the center of the image, surrounded by the verdant foliage.</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> This is a photo of a person in a garden. The person is wearing a gray t-shirt, blue and white swim trunks, and glasses. The person has their hands to their ears. There are many plants and flowers in the garden, and a large tree in the background. The background of the image is blurred. The image is taken from a slightly elevated perspective.</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>surprise</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>0.9078138669331869</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>[    0.21251     0.66714     0.29577     0.31458],[    0.50201     0.41018      0.9868     0.81768]</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>0.5303586, 0.44902265</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>id_1190515268356755461_2019-11-02.jpg</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">person, flower, </t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>there is a man and a woman sitting on a bench</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>In the image, there are two individuals seated on a bench in a garden setting. The person on the left is wearing a black baseball cap and a black t-shirt, while the person on the right is wearing a blue jacket and a gray t-shirt. Both individuals are smiling and looking directly at the camera. The garden around them is lush with greenery, including bushes and flowers, and the sky is visible in the background.</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> This is a photo of Leonardo DiCaprio and Greta Thunberg. They are sitting outdoors. There are plants in the background. They are both smiling. Leonardo DiCaprio is wearing a black cap and a black t-shirt. Greta Thunberg is wearing a blue sweatshirt and a grey t-shirt.</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>disgust</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>0.9079781373341879</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>[    0.29657     0.55917      0.5897      0.8774],[    0.95044     0.49172    0.092934    0.093023]</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>0.4529528, 0.3819592</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>id_1113624374702166017_2019-04-04.jpg</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">person, </t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>someone is making a mess in their house with a cardboard box</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>In the image, a person is standing in a room, holding a piece of wood and preparing to cut it. The person is wearing a black shirt and is positioned in front of a wooden door. The room has a white wall and a wooden floor, creating a contrast between the person's dark clothing and the lighter elements of the room. The person is also holding a piece of paper, possibly a message or instructions.</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> This is a live video of Alexandria Ocasio-Cortez putting together furniture. She is wearing a black long-sleeved shirt and black pants. She is standing in a room that is mostly empty, except for a few pieces of furniture and some boxes. There is a window in the background. The background of the image is a white wall. The setting of the background is indoor. The type of the image is a video.</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>sadness</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>0.8865760962168375</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>[    0.17294     0.49255     0.32297     0.43309]</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>0.4863836</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>id_1207450022591238144_2019-12-18.jpg</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">car, </t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>arafed image of a group of men in suits standing next to a race car</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>In the image, a group of six individuals dressed in formal attire, including black suits and white shirts, are standing in front of a blue and gray race car. The car is parked in a large warehouse-like space, with a high ceiling and large windows that allow natural light to filter in. The individuals are arranged in a line, with the person in the center standing slightly ahead of the others. The background features a large window that offers a view of the sky, adding depth to the scene.</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> There are seven men standing in front of a Formula E race car. The men are all wearing black suits and ties. The car is blue and white. There is a large window in the background. There are also some industrial-looking machines and equipment in the background. The background is dark and shadowy. The image is a photo.</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>0.8991029262542725</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>crowded</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>[    0.32845     0.73155     0.63035     0.25044]</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>0.49228573</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
large-scale changes all around the code
- created noun_count files to analyze nouns for object vocabulary/further analysis
- added GroundingDINO code
- pipeline refactoring
- analyze result excel notebook graphs got rename and code changed
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -486,7 +486,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">poster, </t>
+          <t>poster</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -520,12 +520,12 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[    0.50049     0.50024     0.98844     0.99073]</t>
+          <t>[    0.50035     0.50007     0.98906     0.99065]</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.4777811</t>
+          <t>0.3906828</t>
         </is>
       </c>
     </row>
@@ -535,7 +535,11 @@
           <t>id_1163744643600637952_2019-08-20.jpg</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>snow</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>arafed view of a field with a trail in the snow</t>
@@ -565,8 +569,16 @@
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>[     0.5001     0.78907           1      0.4214]</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0.4067031</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -574,7 +586,11 @@
           <t>id_1122574040936452097_2019-04-28.jpg</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>glacier</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>a close up of a hole in a wall with a black and white dog</t>
@@ -604,8 +620,16 @@
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>[    0.50144     0.47236     0.23467     0.31704]</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0.38370985</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -615,7 +639,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">person, </t>
+          <t>person</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -649,12 +673,12 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>[    0.55928     0.55452     0.47864     0.57719]</t>
+          <t>[    0.55918     0.55452     0.47884     0.57723]</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0.5110339</t>
+          <t>0.47672573</t>
         </is>
       </c>
     </row>
@@ -666,7 +690,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">tree, plant, </t>
+          <t>tree,podium,plant</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -700,12 +724,12 @@
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
-          <t>[     0.4836      0.4533     0.31186     0.37395],[    0.48356     0.45354     0.30985      0.3733]</t>
+          <t>[    0.48386     0.45351     0.31128      0.3735],[    0.72244     0.61256     0.16141     0.14683],[    0.48364     0.45348     0.31012     0.37298]</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0.6861728, 0.43398994</t>
+          <t>0.6849565, 0.5135502, 0.38693547</t>
         </is>
       </c>
     </row>
@@ -717,7 +741,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">person, </t>
+          <t>podium,person,flag</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -751,12 +775,12 @@
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
-          <t>[    0.64667     0.47426     0.59342     0.71294]</t>
+          <t>[    0.18573     0.60911       0.121     0.24808],[    0.64521     0.47421     0.58957     0.71254],[    0.18102     0.42178    0.072017     0.15551]</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>0.51144177</t>
+          <t>0.50541675, 0.4737043, 0.42418364</t>
         </is>
       </c>
     </row>
@@ -768,7 +792,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">poster, </t>
+          <t>glacier,sign,camera,map,mountain,poster</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -806,12 +830,12 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>[    0.25319     0.52039     0.50318     0.94886]</t>
+          <t>[    0.25408     0.51953     0.50421     0.94968],[    0.25361     0.52039     0.50393     0.94866],[    0.84931     0.57744    0.038343    0.066539],[    0.25352     0.52051     0.50352     0.94984],[    0.74161      0.2068     0.47352     0.10733],[    0.25401     0.52041     0.50412      0.9485]</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>0.57296276</t>
+          <t>0.39810526, 0.5070563, 0.41183785, 0.43476003, 0.4302195, 0.45908466</t>
         </is>
       </c>
     </row>
@@ -823,7 +847,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">person, poster, </t>
+          <t>person,book,poster,podium</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -857,12 +881,12 @@
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
-          <t>[    0.48131     0.56876     0.58897     0.85699],[    0.42381     0.18348     0.55205     0.36521]</t>
+          <t>[    0.48141     0.56795     0.58878       0.858],[    0.12911     0.79567     0.25538      0.2004],[    0.42391     0.18381     0.55161     0.36553],[    0.15456       0.798     0.30594     0.39658]</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>0.49001718, 0.38414583</t>
+          <t>0.4189234, 0.39079067, 0.41635087, 0.37884402</t>
         </is>
       </c>
     </row>
@@ -872,11 +896,7 @@
           <t>id_1163810197778903040_2019-08-20.jpg</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">tree, </t>
-        </is>
-      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
           <t>smoke billowing from a forest fire in the middle of the day</t>
@@ -906,16 +926,8 @@
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>[     0.4997     0.75507     0.99399     0.48348]</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>0.41401386</t>
-        </is>
-      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -925,7 +937,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">person, </t>
+          <t>person</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -959,12 +971,12 @@
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr">
         <is>
-          <t>[    0.21827     0.69374     0.43625     0.61303]</t>
+          <t>[    0.21822     0.69391     0.43636     0.61248]</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>0.6026033</t>
+          <t>0.6345378</t>
         </is>
       </c>
     </row>
@@ -976,7 +988,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve">poster, person, </t>
+          <t>map</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1014,12 +1026,12 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>[    0.81833      0.3493     0.23254     0.59861],[     0.5434     0.43226     0.17948     0.30161]</t>
+          <t>[    0.81969     0.34883      0.2358     0.60134]</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>0.4040551, 0.4006823</t>
+          <t>0.4421639</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1043,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve">person, tree, </t>
+          <t>person,tree</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1065,12 +1077,12 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
-          <t>[    0.21251     0.66714     0.29577     0.31458],[    0.50201     0.41018      0.9868     0.81768]</t>
+          <t>[    0.21239     0.66656     0.29598     0.31358],[    0.50171     0.41076     0.98706     0.81836]</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>0.5303586, 0.44902265</t>
+          <t>0.51314807, 0.39316073</t>
         </is>
       </c>
     </row>
@@ -1082,7 +1094,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve">person, flower, </t>
+          <t>person,flower</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1116,12 +1128,12 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
         <is>
-          <t>[    0.29657     0.55917      0.5897      0.8774],[    0.95044     0.49172    0.092934    0.093023]</t>
+          <t>[    0.29658      0.5592     0.58964     0.87699],[     0.9504     0.49174     0.09288    0.093094]</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>0.4529528, 0.3819592</t>
+          <t>0.43543482, 0.37039283</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1145,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve">person, </t>
+          <t>sign,person</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1167,12 +1179,12 @@
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t>[    0.17294     0.49255     0.32297     0.43309]</t>
+          <t>[     0.6372     0.03649     0.12775    0.051663],[    0.16469     0.49228     0.30822     0.43286]</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>0.4863836</t>
+          <t>0.39736262, 0.42133933</t>
         </is>
       </c>
     </row>
@@ -1184,7 +1196,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve">car, </t>
+          <t>car</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1222,12 +1234,12 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>[    0.32845     0.73155     0.63035     0.25044]</t>
+          <t>[    0.32883     0.73569     0.62881     0.24144]</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>0.49228573</t>
+          <t>0.40813386</t>
         </is>
       </c>
     </row>

</xml_diff>